<commit_message>
Removed knock outs in iFerment
If Knockouts are handled in iFerment assignments, then they should not be knocked out in iFerment.
</commit_message>
<xml_diff>
--- a/iFermentAsCkluyveri.xlsx
+++ b/iFermentAsCkluyveri.xlsx
@@ -1218,7 +1218,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-0.04461569661326293</v>
+        <v>-0.04461569661326287</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-0.04461569661326292</v>
+        <v>-0.04461569661326287</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.00202798620969376</v>
+        <v>0.002027986209693753</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.00202798620969376</v>
+        <v>0.002027986209693753</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-0.0466436828229567</v>
+        <v>-0.04664368282295666</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-0.9999999999999976</v>
+        <v>-0.9999999999999967</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.9683634151287746</v>
+        <v>0.9683634151287738</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.9237477185155117</v>
+        <v>0.9237477185155109</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.9237477185155116</v>
+        <v>0.9237477185155109</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.9237477185155117</v>
+        <v>0.9237477185155107</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1.608598661529098</v>
+        <v>1.608598661529096</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0.05576962076657865</v>
+        <v>0.05576962076657832</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>0.03285337659703792</v>
+        <v>0.03285337659703828</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.06814033664570951</v>
+        <v>0.06814033664570983</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-3.369701886027168</v>
+        <v>-4.549381464206029</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>3.369701886027168</v>
+        <v>4.549381464206029</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.4295274792131411</v>
+        <v>0.4295274792131408</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1.341798780517425e-16</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>1.011871212050678e-16</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>1.011871212050678e-16</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1906,7 +1906,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>3.422023930237267</v>
+        <v>4.601703508416128</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1938,7 +1938,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>2.171973230582027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2050,7 +2050,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>0.4295274792131411</v>
+        <v>0.4295274792131407</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2058,7 +2058,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>0.2147637396065706</v>
+        <v>-0.9649158385722943</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2066,7 +2066,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>-3.344960454268904</v>
+        <v>-3.3449604542689</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2074,7 +2074,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>3.344960454268904</v>
+        <v>3.3449604542689</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2082,7 +2082,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>0.9588318799432121</v>
+        <v>0.9588318799432112</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2090,7 +2090,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>-0.6546339484891495</v>
+        <v>-0.654633948489149</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2098,7 +2098,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>0.6546339484891495</v>
+        <v>0.654633948489149</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2122,7 +2122,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>0.1423646319205026</v>
+        <v>0.1423646319205023</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2130,7 +2130,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>0.1423646319205026</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>0.1423646319205023</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>0.04502129385520167</v>
+        <v>0.04502129385520163</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2170,7 +2170,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>0.04502129385520164</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2194,7 +2194,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>7.509768303535663e-17</v>
+        <v>3.152381414159282e-16</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2202,7 +2202,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>0</v>
+        <v>2.359359156357729</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2210,7 +2210,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>-1.048874467653617</v>
+        <v>-1.048874467653616</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2218,7 +2218,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>1.048874467653617</v>
+        <v>1.048874467653616</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2226,7 +2226,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>-0.0255526262421415</v>
+        <v>-0.02555262624214147</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2234,7 +2234,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>0.02555262624214149</v>
+        <v>0.02555262624214147</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2242,7 +2242,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>0.2261204623808553</v>
+        <v>0.2261204623808548</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2250,7 +2250,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>0.5767592780369081</v>
+        <v>0.5767592780369075</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2258,7 +2258,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>-0.1046440884201997</v>
+        <v>-0.1046440884201996</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2266,7 +2266,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>0.1046440884201997</v>
+        <v>0.1046440884201996</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>0.1216791725816262</v>
+        <v>0.121679172581626</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>0.1216791725816262</v>
+        <v>0.1216791725816261</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2314,7 +2314,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>0.06814033664570951</v>
+        <v>0.06814033664570983</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2506,7 +2506,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>0.8906915432975026</v>
+        <v>0.8906915432975013</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2610,7 +2610,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>4.165686473331973</v>
+        <v>5.345366051510833</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>-4.380450212938541</v>
+        <v>-4.380450212938538</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2698,7 +2698,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>-0.3930237274386525</v>
+        <v>-0.393023727438652</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2722,7 +2722,7 @@
         <v>201</v>
       </c>
       <c r="B202">
-        <v>0</v>
+        <v>-1.011871212050678e-16</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2730,7 +2730,7 @@
         <v>202</v>
       </c>
       <c r="B203">
-        <v>0</v>
+        <v>1.011871212050678e-16</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2738,7 +2738,7 @@
         <v>203</v>
       </c>
       <c r="B204">
-        <v>0</v>
+        <v>1.011871212050678e-16</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2746,7 +2746,7 @@
         <v>204</v>
       </c>
       <c r="B205">
-        <v>0</v>
+        <v>1.011871212050678e-16</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2770,7 +2770,7 @@
         <v>207</v>
       </c>
       <c r="B208">
-        <v>-3.422023930237267</v>
+        <v>-4.601703508416128</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2786,7 +2786,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>0.9999999999999973</v>
+        <v>0.9999999999999966</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2794,7 +2794,7 @@
         <v>210</v>
       </c>
       <c r="B211">
-        <v>0</v>
+        <v>-1.011871212050678e-16</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -3026,7 +3026,7 @@
         <v>239</v>
       </c>
       <c r="B240">
-        <v>0.1423646319205026</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -3034,7 +3034,7 @@
         <v>240</v>
       </c>
       <c r="B241">
-        <v>0.04502129385520168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -3042,7 +3042,7 @@
         <v>241</v>
       </c>
       <c r="B242">
-        <v>2.171973230582027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:2">

</xml_diff>

<commit_message>
Revert "Removed knock outs in iFerment"
This reverts commit ef58ca7f80cbcea592b2c891294b126010318fa2.
</commit_message>
<xml_diff>
--- a/iFermentAsCkluyveri.xlsx
+++ b/iFermentAsCkluyveri.xlsx
@@ -1218,7 +1218,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-0.04461569661326287</v>
+        <v>-0.04461569661326293</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-0.04461569661326287</v>
+        <v>-0.04461569661326292</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.002027986209693753</v>
+        <v>0.00202798620969376</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.002027986209693753</v>
+        <v>0.00202798620969376</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-0.04664368282295666</v>
+        <v>-0.0466436828229567</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-0.9999999999999967</v>
+        <v>-0.9999999999999976</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.9683634151287738</v>
+        <v>0.9683634151287746</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.9237477185155109</v>
+        <v>0.9237477185155117</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.9237477185155109</v>
+        <v>0.9237477185155116</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.9237477185155107</v>
+        <v>0.9237477185155117</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1.608598661529096</v>
+        <v>1.608598661529098</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0.05576962076657832</v>
+        <v>0.05576962076657865</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>0.03285337659703828</v>
+        <v>0.03285337659703792</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.06814033664570983</v>
+        <v>0.06814033664570951</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-4.549381464206029</v>
+        <v>-3.369701886027168</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>4.549381464206029</v>
+        <v>3.369701886027168</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.4295274792131408</v>
+        <v>0.4295274792131411</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>1.341798780517425e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>1.011871212050678e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>1.011871212050678e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1906,7 +1906,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>4.601703508416128</v>
+        <v>3.422023930237267</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1938,7 +1938,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>2.171973230582027</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2050,7 +2050,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>0.4295274792131407</v>
+        <v>0.4295274792131411</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2058,7 +2058,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>-0.9649158385722943</v>
+        <v>0.2147637396065706</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2066,7 +2066,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>-3.3449604542689</v>
+        <v>-3.344960454268904</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2074,7 +2074,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>3.3449604542689</v>
+        <v>3.344960454268904</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2082,7 +2082,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>0.9588318799432112</v>
+        <v>0.9588318799432121</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2090,7 +2090,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>-0.654633948489149</v>
+        <v>-0.6546339484891495</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2098,7 +2098,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>0.654633948489149</v>
+        <v>0.6546339484891495</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2122,7 +2122,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>0.1423646319205023</v>
+        <v>0.1423646319205026</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2130,7 +2130,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>0</v>
+        <v>0.1423646319205026</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>0.1423646319205023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>0.04502129385520163</v>
+        <v>0.04502129385520167</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2170,7 +2170,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>0.04502129385520164</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2194,7 +2194,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>3.152381414159282e-16</v>
+        <v>7.509768303535663e-17</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2202,7 +2202,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>2.359359156357729</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2210,7 +2210,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>-1.048874467653616</v>
+        <v>-1.048874467653617</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2218,7 +2218,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>1.048874467653616</v>
+        <v>1.048874467653617</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2226,7 +2226,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>-0.02555262624214147</v>
+        <v>-0.0255526262421415</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2234,7 +2234,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>0.02555262624214147</v>
+        <v>0.02555262624214149</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2242,7 +2242,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>0.2261204623808548</v>
+        <v>0.2261204623808553</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2250,7 +2250,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>0.5767592780369075</v>
+        <v>0.5767592780369081</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2258,7 +2258,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>-0.1046440884201996</v>
+        <v>-0.1046440884201997</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2266,7 +2266,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>0.1046440884201996</v>
+        <v>0.1046440884201997</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>0.121679172581626</v>
+        <v>0.1216791725816262</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>0.1216791725816261</v>
+        <v>0.1216791725816262</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2314,7 +2314,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>0.06814033664570983</v>
+        <v>0.06814033664570951</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2506,7 +2506,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>0.8906915432975013</v>
+        <v>0.8906915432975026</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2610,7 +2610,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>5.345366051510833</v>
+        <v>4.165686473331973</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>-4.380450212938538</v>
+        <v>-4.380450212938541</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2698,7 +2698,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>-0.393023727438652</v>
+        <v>-0.3930237274386525</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2722,7 +2722,7 @@
         <v>201</v>
       </c>
       <c r="B202">
-        <v>-1.011871212050678e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2730,7 +2730,7 @@
         <v>202</v>
       </c>
       <c r="B203">
-        <v>1.011871212050678e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2738,7 +2738,7 @@
         <v>203</v>
       </c>
       <c r="B204">
-        <v>1.011871212050678e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2746,7 +2746,7 @@
         <v>204</v>
       </c>
       <c r="B205">
-        <v>1.011871212050678e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2770,7 +2770,7 @@
         <v>207</v>
       </c>
       <c r="B208">
-        <v>-4.601703508416128</v>
+        <v>-3.422023930237267</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2786,7 +2786,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>0.9999999999999966</v>
+        <v>0.9999999999999973</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2794,7 +2794,7 @@
         <v>210</v>
       </c>
       <c r="B211">
-        <v>-1.011871212050678e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -3026,7 +3026,7 @@
         <v>239</v>
       </c>
       <c r="B240">
-        <v>0</v>
+        <v>0.1423646319205026</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -3034,7 +3034,7 @@
         <v>240</v>
       </c>
       <c r="B241">
-        <v>0</v>
+        <v>0.04502129385520168</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -3042,7 +3042,7 @@
         <v>241</v>
       </c>
       <c r="B242">
-        <v>0</v>
+        <v>2.171973230582027</v>
       </c>
     </row>
     <row r="243" spans="1:2">

</xml_diff>